<commit_message>
Inhouse Review 2 Completed
</commit_message>
<xml_diff>
--- a/Data/Xero_Config.xlsx
+++ b/Data/Xero_Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SodiqBakare\Documents\UiPath\UIPATH\Xero_Project\Xero_Bank_Recon_Deluxe\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kanayo.Eruchalu\Documents\UiPath\Xero_Bank_Recon_Deluxe\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83EA0869-C76F-47D2-AAA0-F6187DB0A077}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{506C6D0A-0E2C-4396-A8DE-C0551D68854D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="493" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="63">
   <si>
     <t>Name</t>
   </si>
@@ -208,6 +208,12 @@
   </si>
   <si>
     <t>EXTERNAL CONFIG FILE</t>
+  </si>
+  <si>
+    <t>XeroDashboardUrl</t>
+  </si>
+  <si>
+    <t>https://go.xero.com/Dashboard/default.aspx</t>
   </si>
 </sst>
 </file>
@@ -593,10 +599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z956"/>
+  <dimension ref="A1:Z957"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -681,8 +687,12 @@
       <c r="Z3" s="1"/>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-      <c r="B4" s="10"/>
+      <c r="A4" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>62</v>
+      </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -708,188 +718,215 @@
       <c r="Y4" s="1"/>
       <c r="Z4" s="1"/>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="11" t="s">
+    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1"/>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8"/>
+      <c r="B6" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="8"/>
-    </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>20</v>
-      </c>
+      <c r="C6" s="8"/>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B8" s="9" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B9" s="9" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>39</v>
+        <v>54</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>19</v>
+        <v>55</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B13" s="15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="7"/>
-    </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="11" t="s">
+    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="7"/>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
+      <c r="B17" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="8"/>
-    </row>
-    <row r="17" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="C17" s="8"/>
+    </row>
+    <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B18" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B19" s="9" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>42</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B20" s="9" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+    <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B21" s="14" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+    <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B22" s="15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+    <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B23" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+    <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B24" s="15" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+    <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B24" s="14" t="s">
+      <c r="B25" s="14" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+    <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="14" t="s">
+      <c r="B26" s="14" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+    <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="B27" s="15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+    <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B28" s="15" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+    <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B29" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+    <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B30" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1814,6 +1851,7 @@
     <row r="954" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="955" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="956" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="957" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated For Demo 2
</commit_message>
<xml_diff>
--- a/Data/Xero_Config.xlsx
+++ b/Data/Xero_Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kanayo.Eruchalu\Documents\UiPath\Xero_Bank_Recon_Deluxe\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SodiqBakare\Documents\UiPath\UIPATH\Xero_Project\Xero_Bank_Recon_Deluxe\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{506C6D0A-0E2C-4396-A8DE-C0551D68854D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{605DC153-FEB1-47F9-8E3B-6E3DC0B99FFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="493" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="62">
   <si>
     <t>Name</t>
   </si>
@@ -114,9 +114,6 @@
     <t>XeroBR_ExceptionFolderPath</t>
   </si>
   <si>
-    <t>Xero_LoginCredentials</t>
-  </si>
-  <si>
     <t>SheetName_SystemData</t>
   </si>
   <si>
@@ -210,10 +207,10 @@
     <t>EXTERNAL CONFIG FILE</t>
   </si>
   <si>
-    <t>XeroDashboardUrl</t>
-  </si>
-  <si>
-    <t>https://go.xero.com/Dashboard/default.aspx</t>
+    <t>Xero_LoginCredentials_Self</t>
+  </si>
+  <si>
+    <t>https://login.xero.com</t>
   </si>
 </sst>
 </file>
@@ -602,13 +599,13 @@
   <dimension ref="A1:Z957"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.5703125" customWidth="1"/>
-    <col min="2" max="2" width="34.5703125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="41.28515625" style="9" customWidth="1"/>
     <col min="3" max="3" width="53.85546875" customWidth="1"/>
     <col min="4" max="26" width="8.5703125" customWidth="1"/>
   </cols>
@@ -659,7 +656,7 @@
         <v>25</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -688,10 +685,10 @@
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>61</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>62</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -749,13 +746,13 @@
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C6" s="8"/>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>20</v>
@@ -763,39 +760,39 @@
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>19</v>
@@ -803,7 +800,7 @@
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B13" s="15" t="s">
         <v>14</v>
@@ -817,45 +814,45 @@
     <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C17" s="8"/>
     </row>
     <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>33</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B22" s="15" t="s">
         <v>15</v>
@@ -863,7 +860,7 @@
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B23" s="15" t="s">
         <v>19</v>
@@ -871,7 +868,7 @@
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B24" s="15" t="s">
         <v>14</v>
@@ -879,23 +876,23 @@
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B27" s="15" t="s">
         <v>15</v>
@@ -903,7 +900,7 @@
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B28" s="15" t="s">
         <v>19</v>
@@ -911,7 +908,7 @@
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>14</v>
@@ -919,10 +916,10 @@
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3060,7 +3057,7 @@
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
Updated For Demo 3/6/2021
</commit_message>
<xml_diff>
--- a/Data/Xero_Config.xlsx
+++ b/Data/Xero_Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SodiqBakare\Documents\UiPath\UIPATH\Xero_Project\Xero_Bank_Recon_Deluxe\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{605DC153-FEB1-47F9-8E3B-6E3DC0B99FFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{194E4220-0D28-40C3-99F4-F886374AD89E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="493" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -78,12 +78,6 @@
     <t>ExpectionFolderPath</t>
   </si>
   <si>
-    <t>ProcessDataExcelFilePath</t>
-  </si>
-  <si>
-    <t>XeroBR_ProcessDataExcelFilePath</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
@@ -207,10 +201,16 @@
     <t>EXTERNAL CONFIG FILE</t>
   </si>
   <si>
-    <t>Xero_LoginCredentials_Self</t>
-  </si>
-  <si>
     <t>https://login.xero.com</t>
+  </si>
+  <si>
+    <t>XeroBR_ExternalConfigPathFile</t>
+  </si>
+  <si>
+    <t>ExternalConfigPathFile</t>
+  </si>
+  <si>
+    <t>Xero_LoginCredentials_self</t>
   </si>
 </sst>
 </file>
@@ -599,7 +599,7 @@
   <dimension ref="A1:Z957"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -647,16 +647,16 @@
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
       <c r="B2" s="11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C2" s="8"/>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -685,10 +685,10 @@
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -746,61 +746,61 @@
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C6" s="8"/>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B13" s="15" t="s">
         <v>14</v>
@@ -814,45 +814,45 @@
     <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C17" s="8"/>
     </row>
     <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B22" s="15" t="s">
         <v>15</v>
@@ -860,15 +860,15 @@
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B24" s="15" t="s">
         <v>14</v>
@@ -876,23 +876,23 @@
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B27" s="15" t="s">
         <v>15</v>
@@ -900,15 +900,15 @@
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>14</v>
@@ -916,10 +916,10 @@
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2939,7 +2939,7 @@
   <dimension ref="A1:Z958"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3041,26 +3041,26 @@
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3068,15 +3068,15 @@
         <v>16</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>60</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated Ready Demo 3/6/2021
</commit_message>
<xml_diff>
--- a/Data/Xero_Config.xlsx
+++ b/Data/Xero_Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SodiqBakare\Documents\UiPath\UIPATH\Xero_Project\Xero_Bank_Recon_Deluxe\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{194E4220-0D28-40C3-99F4-F886374AD89E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A1EB04D-722E-4F4E-ADB1-EAFAB78A13DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="493" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="493" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="67">
   <si>
     <t>Name</t>
   </si>
@@ -81,9 +81,6 @@
     <t>A</t>
   </si>
   <si>
-    <t>System_Data</t>
-  </si>
-  <si>
     <t>XeroBR_ProcessingFolderPath</t>
   </si>
   <si>
@@ -211,6 +208,24 @@
   </si>
   <si>
     <t>Xero_LoginCredentials_self</t>
+  </si>
+  <si>
+    <t>SystemSetting</t>
+  </si>
+  <si>
+    <t>Bank Reconcilliation Url</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The processing folder path  set in orchestrator Asset </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Arcive  folder path  set in orchestrator Asset </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Expection folder path  set in orchestrator Asset </t>
+  </si>
+  <si>
+    <t xml:space="preserve">The External  folder path  set in orchestrator Asset </t>
   </si>
 </sst>
 </file>
@@ -598,8 +613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z957"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -647,16 +662,16 @@
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
       <c r="B2" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" s="8"/>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -685,10 +700,10 @@
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -746,53 +761,53 @@
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C6" s="8"/>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>18</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>17</v>
@@ -800,7 +815,7 @@
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B13" s="15" t="s">
         <v>14</v>
@@ -814,45 +829,45 @@
     <row r="17" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
       <c r="B17" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C17" s="8"/>
     </row>
     <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>30</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B22" s="15" t="s">
         <v>15</v>
@@ -860,7 +875,7 @@
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B23" s="15" t="s">
         <v>17</v>
@@ -868,7 +883,7 @@
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B24" s="15" t="s">
         <v>14</v>
@@ -876,23 +891,23 @@
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B27" s="15" t="s">
         <v>15</v>
@@ -900,7 +915,7 @@
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B28" s="15" t="s">
         <v>17</v>
@@ -908,7 +923,7 @@
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>14</v>
@@ -916,10 +931,10 @@
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2938,8 +2953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z958"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3041,26 +3056,35 @@
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>23</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3068,15 +3092,21 @@
         <v>16</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated For Demo 4/6/2021
</commit_message>
<xml_diff>
--- a/Data/Xero_Config.xlsx
+++ b/Data/Xero_Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SodiqBakare\Documents\UiPath\UIPATH\Xero_Project\Xero_Bank_Recon_Deluxe\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A1EB04D-722E-4F4E-ADB1-EAFAB78A13DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BCB6AF15-12BF-473A-9019-BAF2A3F5DAF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="493" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="493" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -207,12 +207,6 @@
     <t>ExternalConfigPathFile</t>
   </si>
   <si>
-    <t>Xero_LoginCredentials_self</t>
-  </si>
-  <si>
-    <t>SystemSetting</t>
-  </si>
-  <si>
     <t>Bank Reconcilliation Url</t>
   </si>
   <si>
@@ -226,6 +220,12 @@
   </si>
   <si>
     <t xml:space="preserve">The External  folder path  set in orchestrator Asset </t>
+  </si>
+  <si>
+    <t>Xero_LoginCredentials</t>
+  </si>
+  <si>
+    <t>SystemSettings</t>
   </si>
 </sst>
 </file>
@@ -613,8 +613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z957"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -671,7 +671,7 @@
         <v>22</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -770,7 +770,7 @@
         <v>26</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2953,8 +2953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z958"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3062,7 +3062,7 @@
         <v>23</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3073,7 +3073,7 @@
         <v>18</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3084,7 +3084,7 @@
         <v>24</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3095,7 +3095,7 @@
         <v>25</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3106,7 +3106,7 @@
         <v>58</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update for Demo 4/6/2021 4:05
</commit_message>
<xml_diff>
--- a/Data/Xero_Config.xlsx
+++ b/Data/Xero_Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SodiqBakare\Documents\UiPath\UIPATH\Xero_Project\Xero_Bank_Recon_Deluxe\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BCB6AF15-12BF-473A-9019-BAF2A3F5DAF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19B104E3-3639-4F8A-80C4-8220267D217A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="493" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -222,10 +222,10 @@
     <t xml:space="preserve">The External  folder path  set in orchestrator Asset </t>
   </si>
   <si>
-    <t>Xero_LoginCredentials</t>
-  </si>
-  <si>
     <t>SystemSettings</t>
+  </si>
+  <si>
+    <t>Xero_LoginCredentials_self</t>
   </si>
 </sst>
 </file>
@@ -613,8 +613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z957"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -671,7 +671,7 @@
         <v>22</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -770,7 +770,7 @@
         <v>26</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated For Client Demo 7/6/2021
</commit_message>
<xml_diff>
--- a/Data/Xero_Config.xlsx
+++ b/Data/Xero_Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SodiqBakare\Documents\UiPath\UIPATH\Xero_Project\Xero_Bank_Recon_Deluxe\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19B104E3-3639-4F8A-80C4-8220267D217A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD9099B2-0CAD-4616-90C6-65EEBAC4DA58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="493" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -225,7 +225,7 @@
     <t>SystemSettings</t>
   </si>
   <si>
-    <t>Xero_LoginCredentials_self</t>
+    <t>Xero_LoginCredentials</t>
   </si>
 </sst>
 </file>
@@ -614,7 +614,7 @@
   <dimension ref="A1:Z957"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Corrected Organisation Error .Demo Ready 7/6/2021
</commit_message>
<xml_diff>
--- a/Data/Xero_Config.xlsx
+++ b/Data/Xero_Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SodiqBakare\Documents\UiPath\UIPATH\Xero_Project\Xero_Bank_Recon_Deluxe\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD9099B2-0CAD-4616-90C6-65EEBAC4DA58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DAD6A03-E4E1-4507-8BBD-12B10460F470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="493" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -614,7 +614,7 @@
   <dimension ref="A1:Z957"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>